<commit_message>
Optimize GitHub Actions workflow and fix test case
- Add use-public-rspm: true to use pre-compiled binary packages
- Add R package caching to speed up subsequent workflow runs
- Remove redundant direct validation step with old file paths
- Update Excel file fixes test case validation

This reduces workflow runtime from 90+ minutes to ~5-10 minutes.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/inst/testdata/hct_patients.xlsx
+++ b/inst/testdata/hct_patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bill/projects/ohdsi/ohdsi_symposium_2025/cohortTdd.demo/inst/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0C38A3-3398-1745-9889-83FB0477A884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F483319-9CB4-404B-9A53-30E1D0506CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="22220" windowHeight="13680" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6359,7 +6359,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6425,6 +6425,9 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
       <c r="C6" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
purposely break test to check that workflow registers failure
</commit_message>
<xml_diff>
--- a/inst/testdata/hct_patients.xlsx
+++ b/inst/testdata/hct_patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bill/projects/ohdsi/ohdsi_symposium_2025/cohortTdd.demo/inst/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F483319-9CB4-404B-9A53-30E1D0506CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8860499B-28C1-8247-951D-BC1C5681BC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="22220" windowHeight="13680" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6425,9 +6425,6 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
       <c r="C6" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
Resetting purposely failing test - workflow should pass
</commit_message>
<xml_diff>
--- a/inst/testdata/hct_patients.xlsx
+++ b/inst/testdata/hct_patients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bill/projects/ohdsi/ohdsi_symposium_2025/cohortTdd.demo/inst/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8860499B-28C1-8247-951D-BC1C5681BC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08122B48-303B-3547-9258-B686D0103FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="22220" windowHeight="13680" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6425,6 +6425,9 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
       <c r="C6" t="s">
         <v>98</v>
       </c>

</xml_diff>